<commit_message>
Updated test data for Belgium fireclass market
</commit_message>
<xml_diff>
--- a/Test Data/FC_Gallery_Accessories.xlsx
+++ b/Test Data/FC_Gallery_Accessories.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1A24FE-8F89-4475-8343-5C2E115AD3BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B54C70B-EAB9-42EA-95B4-1F629438B016}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Denmark, Sweden and Norway Test data and updated Gallery_Loops_P_Panel and Gallery_Loops_MZX_Panels test data for Swiss, Portugal market and Gallery Panel accessories Pro panels sheet for Slovakia, Czech market
</commit_message>
<xml_diff>
--- a/Test Data/FC_Gallery_Accessories.xlsx
+++ b/Test Data/FC_Gallery_Accessories.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B54C70B-EAB9-42EA-95B4-1F629438B016}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E17C82F-5931-42F5-ABFD-BE05D632D238}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="12" r:id="rId1"/>
     <sheet name="Belgium" sheetId="6" r:id="rId2"/>
+    <sheet name="Denmark" sheetId="13" r:id="rId3"/>
+    <sheet name="Sweden" sheetId="15" r:id="rId4"/>
+    <sheet name="Norway" sheetId="16" r:id="rId5"/>
+    <sheet name="Italy" sheetId="14" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="33">
   <si>
     <t>Wg</t>
   </si>
@@ -109,6 +113,30 @@
   </si>
   <si>
     <t>UK and Turkey Market</t>
+  </si>
+  <si>
+    <t>Denmark Market</t>
+  </si>
+  <si>
+    <t>NGC-3446/T2004</t>
+  </si>
+  <si>
+    <t>FCXB-S</t>
+  </si>
+  <si>
+    <t>Italy Market</t>
+  </si>
+  <si>
+    <t>Sweden market</t>
+  </si>
+  <si>
+    <t>NGC-3465/T2029</t>
+  </si>
+  <si>
+    <t>Norway market</t>
+  </si>
+  <si>
+    <t>NGC-3464/T1918</t>
   </si>
 </sst>
 </file>
@@ -532,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F31FDBE-7B5F-45D2-AA42-DD016472A477}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -820,4 +848,475 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20FC11A3-55D2-4AFC-AB10-43510A3BFCF2}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C363A843-471B-4C73-A7AE-6676E06299BA}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3630B005-044B-4751-B388-D36271E19ADB}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE376BE0-6E42-4AAA-A52A-0260438E9A30}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test data for ItalyFC Market
</commit_message>
<xml_diff>
--- a/Test Data/FC_Gallery_Accessories.xlsx
+++ b/Test Data/FC_Gallery_Accessories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E17C82F-5931-42F5-ABFD-BE05D632D238}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3287AC-9239-4A0B-B582-2622A1976521}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="12" r:id="rId1"/>
@@ -19,6 +19,10 @@
     <sheet name="Sweden" sheetId="15" r:id="rId4"/>
     <sheet name="Norway" sheetId="16" r:id="rId5"/>
     <sheet name="Italy" sheetId="14" r:id="rId6"/>
+    <sheet name="Spain" sheetId="17" r:id="rId7"/>
+    <sheet name="Serbia" sheetId="18" r:id="rId8"/>
+    <sheet name="Romania" sheetId="19" r:id="rId9"/>
+    <sheet name="Slovakia" sheetId="20" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="42">
   <si>
     <t>Wg</t>
   </si>
@@ -124,9 +128,6 @@
     <t>FCXB-S</t>
   </si>
   <si>
-    <t>Italy Market</t>
-  </si>
-  <si>
     <t>Sweden market</t>
   </si>
   <si>
@@ -137,6 +138,36 @@
   </si>
   <si>
     <t>NGC-3464/T1918</t>
+  </si>
+  <si>
+    <t>Italy market</t>
+  </si>
+  <si>
+    <t>NGC-3443/T1916</t>
+  </si>
+  <si>
+    <t>Spain market</t>
+  </si>
+  <si>
+    <t>NGC-3442/T1592</t>
+  </si>
+  <si>
+    <t>Serbia market</t>
+  </si>
+  <si>
+    <t>NGC-4305/T3495</t>
+  </si>
+  <si>
+    <t>Romania market</t>
+  </si>
+  <si>
+    <t>NGC-4307/T3541</t>
+  </si>
+  <si>
+    <t>Slovakia market</t>
+  </si>
+  <si>
+    <t>NGC-4306/T3555</t>
   </si>
 </sst>
 </file>
@@ -703,6 +734,153 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE80CAAC-E5AA-4DF2-A8D4-F9D09AFC5E89}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FB1E1A-05DD-49D0-9147-9D7D528C068A}">
   <dimension ref="A1:D20"/>
@@ -991,7 +1169,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -1013,7 +1191,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">
@@ -1078,7 +1256,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3630B005-044B-4751-B388-D36271E19ADB}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1103,7 +1281,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -1125,7 +1303,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">
@@ -1191,7 +1369,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,7 +1393,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>3</v>
@@ -1236,7 +1414,9 @@
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -1308,6 +1488,437 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85770E7E-DE2B-48E1-8E45-1BA06C4C35B5}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C811BBCD-D5D7-4F56-974F-3CD7556C101B}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1241DB-745A-4E84-AB2D-50C30F7CA44C}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added HungaryFC Test data
</commit_message>
<xml_diff>
--- a/Test Data/FC_Gallery_Accessories.xlsx
+++ b/Test Data/FC_Gallery_Accessories.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3287AC-9239-4A0B-B582-2622A1976521}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9859122F-3CE9-4223-A874-29505DDA5F90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="9" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="10" xr2:uid="{C41C5F48-4FD1-41E2-932B-493D5E69981C}"/>
   </bookViews>
   <sheets>
     <sheet name="UK" sheetId="12" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Serbia" sheetId="18" r:id="rId8"/>
     <sheet name="Romania" sheetId="19" r:id="rId9"/>
     <sheet name="Slovakia" sheetId="20" r:id="rId10"/>
+    <sheet name="Hungary" sheetId="21" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="44">
   <si>
     <t>Wg</t>
   </si>
@@ -168,6 +169,12 @@
   </si>
   <si>
     <t>NGC-4306/T3555</t>
+  </si>
+  <si>
+    <t>Hungary Market</t>
+  </si>
+  <si>
+    <t>NGC-4308/T3599</t>
   </si>
 </sst>
 </file>
@@ -738,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE80CAAC-E5AA-4DF2-A8D4-F9D09AFC5E89}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -786,6 +793,153 @@
       </c>
       <c r="B4" s="3" t="s">
         <v>41</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="6"/>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FCF4CA-1CFF-4A2E-A9C2-CF47A2D41591}">
+  <dimension ref="A1:D20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">

</xml_diff>